<commit_message>
Updated spreadsheet and chart
</commit_message>
<xml_diff>
--- a/SaloniDattani/Antipsychotic-drugs/Psychosis treatments.xlsx
+++ b/SaloniDattani/Antipsychotic-drugs/Psychosis treatments.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="115">
   <si>
     <t>Treatment_name</t>
   </si>
@@ -32,316 +32,319 @@
     <t>Year_first_used_approved_US</t>
   </si>
   <si>
-    <t>Inventor_manufacturer</t>
+    <t>Inventor_manufacturer_first</t>
+  </si>
+  <si>
+    <t>Indications_current</t>
+  </si>
+  <si>
+    <t>Citations_further_reading</t>
+  </si>
+  <si>
+    <t>FDA_label</t>
+  </si>
+  <si>
+    <t>Chlorpromazine</t>
+  </si>
+  <si>
+    <t>Antipsychotic</t>
+  </si>
+  <si>
+    <t>First-generation antipsychotic</t>
+  </si>
+  <si>
+    <t>Phenothiazine</t>
+  </si>
+  <si>
+    <t>Paul Charpentier (original synthesis) / Laborit, Lehmann, and Deniker (credited Lasker prize)</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/16433053/</t>
+  </si>
+  <si>
+    <t>Reserpine</t>
+  </si>
+  <si>
+    <t>Antipsychotic and antihypertensive (natural)</t>
+  </si>
+  <si>
+    <t>Rauwolfia alkaloid</t>
+  </si>
+  <si>
+    <t>Natural compound in the plant Rauvolfia serpentina; first synthesized by R. B. Woodward in 1958; first licensed as an antihypertensive in 1953 and as a tranquilizer/antipsychotic as 1954</t>
+  </si>
+  <si>
+    <t>https://www.acs.org/molecule-of-the-week/archive/r/reserpine.html</t>
+  </si>
+  <si>
+    <t>Haloperidol</t>
+  </si>
+  <si>
+    <t>Butyrophenone</t>
+  </si>
+  <si>
+    <t>Paul Janssen</t>
+  </si>
+  <si>
+    <t>Schizophrenia; Tourette syndrome (FDA); delirium, bipolar disorder, psychotic symptoms in Alzheimer's, chorea in Huntington's (NICE)</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/16433054/</t>
+  </si>
+  <si>
+    <t>https://www.accessdata.fda.gov/drugsatfda_docs/label/2008/015923s082,018701s057lbl.pdf</t>
+  </si>
+  <si>
+    <t>Fluphenazine</t>
+  </si>
+  <si>
+    <t>Squibb</t>
+  </si>
+  <si>
+    <t>Thioridazine</t>
+  </si>
+  <si>
+    <t>Sandoz</t>
+  </si>
+  <si>
+    <t>Loxapine</t>
+  </si>
+  <si>
+    <t>Dibenzoxazepine</t>
+  </si>
+  <si>
+    <t>Lederle</t>
+  </si>
+  <si>
+    <t>Perphenazine</t>
+  </si>
+  <si>
+    <t>Schering</t>
+  </si>
+  <si>
+    <t>Triflupromazine</t>
+  </si>
+  <si>
+    <t>Thiothixene</t>
+  </si>
+  <si>
+    <t>Thioxanthene</t>
+  </si>
+  <si>
+    <t>Roerig</t>
+  </si>
+  <si>
+    <t>Molindone</t>
+  </si>
+  <si>
+    <t>Dihydroindole</t>
+  </si>
+  <si>
+    <t>Endo</t>
+  </si>
+  <si>
+    <t>Pimozide</t>
+  </si>
+  <si>
+    <t>Diphenylbutylpiperidine</t>
+  </si>
+  <si>
+    <t>Janssen</t>
+  </si>
+  <si>
+    <t>Clozapine</t>
+  </si>
+  <si>
+    <t>Second-generation antipsychotic</t>
+  </si>
+  <si>
+    <t>Wander AG (Swiss pharmaceutical)</t>
+  </si>
+  <si>
+    <t>Treatment-resistant schizophrenia; reducing suicidal behavior</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/17580753/</t>
+  </si>
+  <si>
+    <t>https://www.accessdata.fda.gov/drugsatfda_docs/label/2017/019758s084lbl.pdf</t>
+  </si>
+  <si>
+    <t>Risperidone</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/nrd1062</t>
+  </si>
+  <si>
+    <t>Olanzapine</t>
+  </si>
+  <si>
+    <t>Eli Lilly</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/00325481.2019.1701823</t>
+  </si>
+  <si>
+    <t>Quetiapine</t>
+  </si>
+  <si>
+    <t>AstraZeneca</t>
+  </si>
+  <si>
+    <t>Schizophrenia, bipolar disorder</t>
+  </si>
+  <si>
+    <t>Ziprasidone</t>
+  </si>
+  <si>
+    <t>Pfizer</t>
+  </si>
+  <si>
+    <t>Aripiprazole</t>
+  </si>
+  <si>
+    <t>Third-generation antipsychotic</t>
+  </si>
+  <si>
+    <t>Otsuka Pharmaceutical / Bristol-Myers Squibb</t>
+  </si>
+  <si>
+    <t>Schizophrenia, bipolar mania</t>
+  </si>
+  <si>
+    <t>https://www.accessdata.fda.gov/drugsatfda_docs/label/2005/021713s004,021436s007lbl.pdf</t>
+  </si>
+  <si>
+    <t>Perospirone</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Dainippon Sumitomo Pharma (Japan)</t>
+  </si>
+  <si>
+    <t>Blonaserin</t>
+  </si>
+  <si>
+    <t>Paliperidone</t>
+  </si>
+  <si>
+    <t>Iloperidone</t>
+  </si>
+  <si>
+    <t>Vanda</t>
+  </si>
+  <si>
+    <t>Asenapine</t>
+  </si>
+  <si>
+    <t>Merck</t>
+  </si>
+  <si>
+    <t>Lurasidone</t>
+  </si>
+  <si>
+    <t>Sunovion Pharmaceuticals</t>
+  </si>
+  <si>
+    <t>Cariprazine</t>
+  </si>
+  <si>
+    <t>Allergan</t>
+  </si>
+  <si>
+    <t>Brexpiprazole</t>
+  </si>
+  <si>
+    <t>Otsuka Pharmaceutical / Lundbeck</t>
+  </si>
+  <si>
+    <t>Pimvanserin</t>
+  </si>
+  <si>
+    <t>Acadia Pharmaceutical</t>
+  </si>
+  <si>
+    <t>Lumateperone</t>
+  </si>
+  <si>
+    <t>Bristol Myers Squibb</t>
+  </si>
+  <si>
+    <t>Sertindole</t>
+  </si>
+  <si>
+    <t>Lundbeck / Abbott Laboratories (Czechia, UK)</t>
+  </si>
+  <si>
+    <t>Zotepine</t>
+  </si>
+  <si>
+    <t>Fujisawa (Japan)</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Response_types</t>
+  </si>
+  <si>
+    <t>Column_complete</t>
+  </si>
+  <si>
+    <t>Name of the treatment</t>
+  </si>
+  <si>
+    <t>text, e.g. clozapine</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Type of treatment</t>
+  </si>
+  <si>
+    <t>text, e.g. antipsychotic medication, psychotherapy, surgery, etc.</t>
+  </si>
+  <si>
+    <t>Subtype of treatment</t>
+  </si>
+  <si>
+    <t>text, e.g. second-generation antipsychotic</t>
+  </si>
+  <si>
+    <t>Drug class</t>
+  </si>
+  <si>
+    <t>text, e.g. Phenothiazine</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>The year it was first synthesized or developed in any country</t>
+  </si>
+  <si>
+    <t>numeric, e.g. 1958</t>
+  </si>
+  <si>
+    <t>The year it was first used or approved in the United States (includes pre-FDA uses)</t>
+  </si>
+  <si>
+    <t>numeric, e.g. 1990</t>
+  </si>
+  <si>
+    <t>Name of the scientist, group, company, or institution which is credited with its invention; if unavailable, its first manufacturer</t>
+  </si>
+  <si>
+    <t>text, e.g. Wander AG</t>
   </si>
   <si>
     <t>Indications_current_incomplete</t>
-  </si>
-  <si>
-    <t>Citations_further_reading</t>
-  </si>
-  <si>
-    <t>FDA_label</t>
-  </si>
-  <si>
-    <t>Chlorpromazine</t>
-  </si>
-  <si>
-    <t>Antipsychotic</t>
-  </si>
-  <si>
-    <t>First-generation antipsychotic</t>
-  </si>
-  <si>
-    <t>Phenothiazine</t>
-  </si>
-  <si>
-    <t>Paul Charpentier (original synthesis) / Laborit, Lehmann, and Deniker (credited Lasker prize)</t>
-  </si>
-  <si>
-    <t>https://pubmed.ncbi.nlm.nih.gov/16433053/</t>
-  </si>
-  <si>
-    <t>Reserpine</t>
-  </si>
-  <si>
-    <t>Antipsychotic and antihypertensive (natural)</t>
-  </si>
-  <si>
-    <t>Rauwolfia alkaloid</t>
-  </si>
-  <si>
-    <t>Natural compound in the plant Rauvolfia serpentina; first synthesized by R. B. Woodward in 1958; first licensed as an antihypertensive in 1953 and as a tranquilizer/antipsychotic as 1954</t>
-  </si>
-  <si>
-    <t>https://www.acs.org/molecule-of-the-week/archive/r/reserpine.html</t>
-  </si>
-  <si>
-    <t>Haloperidol</t>
-  </si>
-  <si>
-    <t>Butyrophenone</t>
-  </si>
-  <si>
-    <t>Paul Janssen</t>
-  </si>
-  <si>
-    <t>Schizophrenia; Tourette syndrome (FDA); delirium, bipolar disorder, psychotic symptoms in Alzheimer's, chorea in Huntington's (NICE)</t>
-  </si>
-  <si>
-    <t>https://pubmed.ncbi.nlm.nih.gov/16433054/</t>
-  </si>
-  <si>
-    <t>https://www.accessdata.fda.gov/drugsatfda_docs/label/2008/015923s082,018701s057lbl.pdf</t>
-  </si>
-  <si>
-    <t>Fluphenazine</t>
-  </si>
-  <si>
-    <t>Squibb</t>
-  </si>
-  <si>
-    <t>Thioridazine</t>
-  </si>
-  <si>
-    <t>Sandoz</t>
-  </si>
-  <si>
-    <t>Loxapine</t>
-  </si>
-  <si>
-    <t>Dibenzoxazepine</t>
-  </si>
-  <si>
-    <t>Lederle</t>
-  </si>
-  <si>
-    <t>Perphenazine</t>
-  </si>
-  <si>
-    <t>Schering</t>
-  </si>
-  <si>
-    <t>Triflupromazine</t>
-  </si>
-  <si>
-    <t>Thiothixene</t>
-  </si>
-  <si>
-    <t>Thioxanthene</t>
-  </si>
-  <si>
-    <t>Roerig</t>
-  </si>
-  <si>
-    <t>Molindone</t>
-  </si>
-  <si>
-    <t>Dihydroindole</t>
-  </si>
-  <si>
-    <t>Endo</t>
-  </si>
-  <si>
-    <t>Pimozide</t>
-  </si>
-  <si>
-    <t>Diphenylbutylpiperidine</t>
-  </si>
-  <si>
-    <t>Janssen</t>
-  </si>
-  <si>
-    <t>Clozapine</t>
-  </si>
-  <si>
-    <t>Second-generation antipsychotic</t>
-  </si>
-  <si>
-    <t>Wander AG (Swiss pharmaceutical)</t>
-  </si>
-  <si>
-    <t>Treatment-resistant schizophrenia; reducing suicidal behavior</t>
-  </si>
-  <si>
-    <t>https://pubmed.ncbi.nlm.nih.gov/17580753/</t>
-  </si>
-  <si>
-    <t>https://www.accessdata.fda.gov/drugsatfda_docs/label/2017/019758s084lbl.pdf</t>
-  </si>
-  <si>
-    <t>Risperidone</t>
-  </si>
-  <si>
-    <t>https://www.nature.com/articles/nrd1062</t>
-  </si>
-  <si>
-    <t>Olanzapine</t>
-  </si>
-  <si>
-    <t>Eli Lilly</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1080/00325481.2019.1701823</t>
-  </si>
-  <si>
-    <t>Quetiapine</t>
-  </si>
-  <si>
-    <t>AstraZeneca</t>
-  </si>
-  <si>
-    <t>Schizophrenia, bipolar disorder</t>
-  </si>
-  <si>
-    <t>Ziprasidone</t>
-  </si>
-  <si>
-    <t>Pfizer</t>
-  </si>
-  <si>
-    <t>Aripiprazole</t>
-  </si>
-  <si>
-    <t>Third-generation antipsychotic</t>
-  </si>
-  <si>
-    <t>Otsuka Pharmaceutical / Bristol-Myers Squibb</t>
-  </si>
-  <si>
-    <t>Schizophrenia, bipolar mania</t>
-  </si>
-  <si>
-    <t>https://www.accessdata.fda.gov/drugsatfda_docs/label/2005/021713s004,021436s007lbl.pdf</t>
-  </si>
-  <si>
-    <t>Perospirone</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Dainippon Sumitomo Pharma (Japan)</t>
-  </si>
-  <si>
-    <t>Blonaserin</t>
-  </si>
-  <si>
-    <t>Paliperidone</t>
-  </si>
-  <si>
-    <t>Iloperidone</t>
-  </si>
-  <si>
-    <t>Vanda</t>
-  </si>
-  <si>
-    <t>Asenapine</t>
-  </si>
-  <si>
-    <t>Merck</t>
-  </si>
-  <si>
-    <t>Lurasidone</t>
-  </si>
-  <si>
-    <t>Sunovion Pharmaceuticals</t>
-  </si>
-  <si>
-    <t>Cariprazine</t>
-  </si>
-  <si>
-    <t>Allergan</t>
-  </si>
-  <si>
-    <t>Brexpiprazole</t>
-  </si>
-  <si>
-    <t>Otsuka Pharmaceutical / Lundbeck</t>
-  </si>
-  <si>
-    <t>Pimvanserin</t>
-  </si>
-  <si>
-    <t>Acadia Pharmaceutical</t>
-  </si>
-  <si>
-    <t>Lumateperone</t>
-  </si>
-  <si>
-    <t>Bristol Myers Squibb</t>
-  </si>
-  <si>
-    <t>Sertindole</t>
-  </si>
-  <si>
-    <t>Lundbeck / Abbott Laboratories (Czechia, UK)</t>
-  </si>
-  <si>
-    <t>Zotepine</t>
-  </si>
-  <si>
-    <t>Fujisawa (Japan)</t>
-  </si>
-  <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Response_types</t>
-  </si>
-  <si>
-    <t>Column_complete</t>
-  </si>
-  <si>
-    <t>Name of the treatment</t>
-  </si>
-  <si>
-    <t>text, e.g. clozapine</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Type of treatment</t>
-  </si>
-  <si>
-    <t>text, e.g. antipsychotic medication, psychotherapy, surgery, etc.</t>
-  </si>
-  <si>
-    <t>Subtype of treatment</t>
-  </si>
-  <si>
-    <t>text, e.g. second-generation antipsychotic</t>
-  </si>
-  <si>
-    <t>Drug class</t>
-  </si>
-  <si>
-    <t>text, e.g. Phenothiazine</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>The year it was first synthesized or developed in any country</t>
-  </si>
-  <si>
-    <t>numeric, e.g. 1958</t>
-  </si>
-  <si>
-    <t>The year it was first used or approved in the United States (includes pre-FDA uses)</t>
-  </si>
-  <si>
-    <t>numeric, e.g. 1990</t>
-  </si>
-  <si>
-    <t>Name of the scientist, group, company, or institution which is credited with its invention; if unavailable, its manufacturer</t>
-  </si>
-  <si>
-    <t>text, e.g. Wander AG</t>
   </si>
   <si>
     <t>The names of conditions it is approved to treat currently according to the FDA</t>
@@ -728,9 +731,11 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2"/>
       <c r="E3" s="2">
         <v>1958.0</v>
       </c>
@@ -1439,13 +1444,13 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>103</v>
@@ -1456,10 +1461,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>103</v>
@@ -1470,10 +1475,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>103</v>

</xml_diff>